<commit_message>
paralelizacion solo por proyectos
</commit_message>
<xml_diff>
--- a/Plantilla para entrada.xlsx
+++ b/Plantilla para entrada.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ep_jbarrientost\OneDrive - Colbun S.A\Escritorio\Programa Calculo PPA V2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miuandescl-my.sharepoint.com/personal/jpbarrientos_miuandes_cl/Documents/Escritorio/Programa-Calculo-PPA/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_AA28712D30E3F34326A61B970B3FBC3E0F4BC1D3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFA95AB0-7678-4DBA-A4AF-5F0E8F30DD8B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vector Entrada" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="563">
   <si>
     <t>Nombre Proyecto</t>
   </si>
@@ -1714,18 +1715,12 @@
   </si>
   <si>
     <t xml:space="preserve">Barra retiro (si no hay, dejar en blanco) </t>
-  </si>
-  <si>
-    <t>Opex [MMUSD] (si no hay dejar en blanco) Año 31</t>
-  </si>
-  <si>
-    <t>Terrenos [MMUSD] (si no hay dejar en blanco, solo si no hay opex tabla) Año 31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2047,11 +2042,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A367"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A345" workbookViewId="0">
-      <selection sqref="A1:A367"/>
+    <sheetView tabSelected="1" topLeftCell="A324" workbookViewId="0">
+      <selection activeCell="A336" sqref="A336:XFD336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3736,162 +3731,152 @@
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>563</v>
+        <v>333</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" t="s">
         <v>362</v>
-      </c>
-    </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" t="s">
-        <v>564</v>
       </c>
     </row>
   </sheetData>
@@ -3903,11 +3888,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A248"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5161,14 +5146,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="cea54273-e3dd-4e83-abd0-36ebfa24cb01" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5177,7 +5154,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B95A9644F3155A4791D9A98C28A15B54" ma:contentTypeVersion="6" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="cb67131c7af984eadd5010289ae2ed62">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cea54273-e3dd-4e83-abd0-36ebfa24cb01" xmlns:ns4="38a11414-a502-4b4a-9f4d-78b867b97e86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cf4efdbee7b2474e9093e00599fdf2de" ns3:_="" ns4:_="">
     <xsd:import namespace="cea54273-e3dd-4e83-abd0-36ebfa24cb01"/>
@@ -5354,24 +5331,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5834B42-4824-4AD0-9F69-BBAEAC96AD79}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="38a11414-a502-4b4a-9f4d-78b867b97e86"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cea54273-e3dd-4e83-abd0-36ebfa24cb01"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="cea54273-e3dd-4e83-abd0-36ebfa24cb01" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62644994-A6D8-4C58-8F32-95D7157D5DC8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -5379,7 +5347,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B2C030F-B1FF-40FD-B1AF-B7EAEA038421}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5396,4 +5364,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5834B42-4824-4AD0-9F69-BBAEAC96AD79}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="38a11414-a502-4b4a-9f4d-78b867b97e86"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cea54273-e3dd-4e83-abd0-36ebfa24cb01"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>